<commit_message>
update December 12, 2018 after sending extended work timeline
</commit_message>
<xml_diff>
--- a/experiments/data/flight_costs.xlsx
+++ b/experiments/data/flight_costs.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21045" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21045" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="flight_costs" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$T$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$D$73</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1156,23 +1156,19 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg2"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="90000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>flight_costs!$B$1:$F$1</c:f>
+              <c:f>flight_costs!$B$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Linear
 Importance</c:v>
@@ -1192,16 +1188,26 @@
                 <c:pt idx="4">
                   <c:v>DiVE
 dSwap</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DiVE
+Greedy
+Adaptive</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DiVE
+dSwap
+Adaptive</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flight_costs!$B$2:$F$2</c:f>
+              <c:f>flight_costs!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>12.325840473175026</c:v>
                 </c:pt>
@@ -1216,91 +1222,25 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.325840473175026</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8572906970976995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0257290697097652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2D1B-44A5-8587-9B3AF4BBE606}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>flight_costs!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>flight_costs!$B$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Linear
-Importance</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Greedy
-Diversity</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DiVE
-Greedy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>DiVE
-iSwap</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DiVE
-dSwap</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>flight_costs!#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2D1B-44A5-8587-9B3AF4BBE606}"/>
+              <c16:uniqueId val="{00000000-A5D6-4F26-85BE-D3EF395F7C15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>flight_costs!$A$3</c:f>
@@ -1317,18 +1257,16 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>flight_costs!$B$1:$F$1</c:f>
+              <c:f>flight_costs!$B$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Linear
 Importance</c:v>
@@ -1348,16 +1286,26 @@
                 <c:pt idx="4">
                   <c:v>DiVE
 dSwap</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DiVE
+Greedy
+Adaptive</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DiVE
+dSwap
+Adaptive</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flight_costs!$B$3:$F$3</c:f>
+              <c:f>flight_costs!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1372,13 +1320,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.1594267994812242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35439526824974699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.19942679948122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2D1B-44A5-8587-9B3AF4BBE606}"/>
+              <c16:uniqueId val="{00000001-A5D6-4F26-85BE-D3EF395F7C15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1390,7 +1344,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="92"/>
         <c:overlap val="100"/>
         <c:axId val="468812048"/>
         <c:axId val="468811392"/>
@@ -1419,7 +1373,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1476,8 +1430,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.2989616813831503E-2"/>
-              <c:y val="0.26928917805983194"/>
+              <c:x val="1.6540595408999288E-2"/>
+              <c:y val="0.23716487330014377"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1522,7 +1476,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1547,15 +1501,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30524639655247954"/>
-          <c:y val="0.88455471095417459"/>
-          <c:w val="0.35741400493093844"/>
-          <c:h val="0.11516258384368623"/>
+          <c:x val="7.001339963571028E-2"/>
+          <c:y val="1.4649685079834055E-2"/>
+          <c:w val="0.89999994199620059"/>
+          <c:h val="0.10679430612367839"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1571,7 +1525,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="3500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1610,7 +1564,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.74803149606299213" l="0.70866141732283472" r="0.70866141732283472" t="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2745,20 +2699,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3043,7 +2997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -3146,14 +3100,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <printOptions headings="1" gridLines="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>